<commit_message>
individual z-score and sem-score histograms
</commit_message>
<xml_diff>
--- a/output/supplemental_figures/edge_method/by_implant/implant_test_results.xlsx
+++ b/output/supplemental_figures/edge_method/by_implant/implant_test_results.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="87">
   <si>
     <t>Row</t>
   </si>
@@ -294,7 +294,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -304,14 +304,18 @@
     </border>
     <border/>
     <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -337,364 +341,364 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="3" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="1" t="s">
+      <c r="H3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="1" t="s">
+      <c r="D4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J4" s="1" t="s">
+      <c r="I4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="B5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="1" t="s">
+      <c r="F5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5" s="1" t="s">
+      <c r="H5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="3" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="1" t="s">
+      <c r="B6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I6" s="1" t="s">
+      <c r="H6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="J6" s="3" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="B7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J7" s="1" t="s">
+      <c r="H7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" s="3" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="I9" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="J9" s="3" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I10" s="1" t="s">
+      <c r="H10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="J10" s="3" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G11" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I11" s="1" t="s">
+      <c r="H11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="J11" s="3" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G12" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="H12" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="I12" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="J12" s="3" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G13" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="H13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J13" s="1" t="s">
+      <c r="H13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J13" s="3" t="s">
         <v>86</v>
       </c>
     </row>

</xml_diff>

<commit_message>
p-value and distance visualization
</commit_message>
<xml_diff>
--- a/output/supplemental_figures/edge_method/by_implant/implant_test_results.xlsx
+++ b/output/supplemental_figures/edge_method/by_implant/implant_test_results.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="87">
   <si>
     <t>Row</t>
   </si>
@@ -294,7 +294,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -306,16 +306,28 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -341,364 +353,364 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="9" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="3" t="s">
+      <c r="H3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="9" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="B4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="3" t="s">
+      <c r="D4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J4" s="3" t="s">
+      <c r="I4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="9" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="3" t="s">
+      <c r="B5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="3" t="s">
+      <c r="F5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="H5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5" s="3" t="s">
+      <c r="H5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="9" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="B6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="H6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I6" s="3" t="s">
+      <c r="H6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="J6" s="9" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="B7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="H7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J7" s="3" t="s">
+      <c r="H7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" s="9" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="I9" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="J9" s="3" t="s">
+      <c r="J9" s="9" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="H10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I10" s="3" t="s">
+      <c r="H10" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="J10" s="3" t="s">
+      <c r="J10" s="9" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="H11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I11" s="3" t="s">
+      <c r="H11" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="J11" s="3" t="s">
+      <c r="J11" s="9" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="H12" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="I12" s="3" t="s">
+      <c r="I12" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="J12" s="3" t="s">
+      <c r="J12" s="9" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="G13" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="H13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J13" s="3" t="s">
+      <c r="H13" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J13" s="9" t="s">
         <v>86</v>
       </c>
     </row>

</xml_diff>